<commit_message>
MALS-222 licence expiry report
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Client_Details_Template.xlsx
+++ b/app/server/static/templates/reports/Client_Details_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philarctander/Data/PARC_OD_20210825/PARC Systems Inc/Projects - Documents/MALS/CDOGS/Development/MALS_Templates/Reports/Client_Company_Details/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4B890B-ECE2-A949-806E-22EFECF40574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2A5572-C6B1-4369-B9F6-07B5972F6039}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17040" yWindow="-23620" windowWidth="33220" windowHeight="19640" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Client Details" sheetId="1" r:id="rId1"/>
@@ -110,30 +110,6 @@
     <t>{d.Client[i].LicenceNumber}</t>
   </si>
   <si>
-    <t>{d.Client[i]LicenceHolderCompany}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Address}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]City} {d.Client[i]Province}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Postcode}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Phone}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Fax}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Cell}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Email}</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -146,52 +122,76 @@
     <t>DISPENSER DETAILS</t>
   </si>
   <si>
-    <t>{d.Client[i]DispenserAddress}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]DispenserCity} {d.Client[i]DispenserProvince}</t>
-  </si>
-  <si>
     <t>DISPENSER LICENSES</t>
   </si>
   <si>
-    <t>{d.Client[i]DispenserPostcode}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]IssueDate}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]ExpiryDate}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]Fee}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Disp[i]DispLicense}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Disp[i]DispSurname}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Disp[i]DispGivenName}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Disp[i]DispExpiryDate}</t>
-  </si>
-  <si>
-    <t>{d.Client[i].Disp[i+1]DispLicense}</t>
-  </si>
-  <si>
     <t>{d.Client[i+1].LicenceNumber}</t>
   </si>
   <si>
     <t>-----------------------------------------</t>
   </si>
   <si>
-    <t>{d.Client[i]SiteInspectionDate}</t>
-  </si>
-  <si>
-    <t>{d.Client[i]SiteInspector}</t>
+    <t>{d.Client[i].Address}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].City} {d.Client[i].Province}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Postcode}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Phone}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Fax}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Cell}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Email}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].ExpiryDate}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].SiteInspector}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].IssueDate}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Fee}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].SiteInspectionDate}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].LicenceHolderCompany}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].DispenserAddress}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].DispenserPostcode}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].DispenserCity} {d.Client[i].DispenserProvince}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Disp[i].DispLicense}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Disp[i].DispSurname}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Disp[i].DispGivenName}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Disp[i].DispExpiryDate}</t>
+  </si>
+  <si>
+    <t>{d.Client[i].Disp[i+1].DispLicense}</t>
   </si>
 </sst>
 </file>
@@ -653,21 +653,21 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
@@ -679,7 +679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
@@ -690,13 +690,13 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -724,12 +724,12 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -738,7 +738,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -748,7 +748,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -758,63 +758,63 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="4"/>
       <c r="E12" s="5"/>
@@ -822,7 +822,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -832,7 +832,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -843,47 +843,47 @@
         <v>13</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="28"/>
       <c r="C16" s="1"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -891,35 +891,35 @@
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="4"/>
       <c r="C24" s="21"/>
@@ -927,9 +927,9 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="21"/>
@@ -937,7 +937,7 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>16</v>
       </c>
@@ -953,25 +953,25 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -979,7 +979,7 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="7"/>
       <c r="C29" s="9"/>
@@ -987,35 +987,35 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="F30" s="29" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="22" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1025,21 +1025,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -1262,32 +1247,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61301E0F-7DFD-482F-A08F-018699F653D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D289B0C4-E331-440B-B112-FFBF91054E2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{549ABEF3-110A-4A0B-99BE-4ABD4762681B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1304,4 +1279,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61301E0F-7DFD-482F-A08F-018699F653D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D289B0C4-E331-440B-B112-FFBF91054E2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MALS-1129 Rename 'Dispenser Details' to 'Details'
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Client_Details_Template.xlsx
+++ b/app/server/static/templates/reports/Client_Details_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325B72E0-3C5C-419F-978C-FA370B6D986C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B93F0-95F0-4B89-B037-749AA5BB13C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>Postcode</t>
   </si>
   <si>
-    <t>DISPENSER DETAILS</t>
-  </si>
-  <si>
     <t>DISPENSER LICENSES</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>DETAILS</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -729,7 +729,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -763,19 +763,19 @@
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -785,19 +785,19 @@
         <v>25</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -807,7 +807,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="3"/>
@@ -837,13 +837,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="18"/>
@@ -867,13 +867,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -896,7 +896,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -904,7 +904,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -912,7 +912,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -929,7 +929,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="21"/>
@@ -955,23 +955,23 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
         <v>47</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>48</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>49</v>
-      </c>
-      <c r="D27" t="s">
-        <v>50</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -989,33 +989,33 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B32" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1025,15 +1025,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -1256,6 +1247,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1263,14 +1263,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61301E0F-7DFD-482F-A08F-018699F653D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{549ABEF3-110A-4A0B-99BE-4ABD4762681B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1285,6 +1277,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61301E0F-7DFD-482F-A08F-018699F653D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>